<commit_message>
finished the client class with the
</commit_message>
<xml_diff>
--- a/isd_project/tests/A01_pixell_test_plan_client.xlsx
+++ b/isd_project/tests/A01_pixell_test_plan_client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27728"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dkwarkentin\Documents\Course Folders\2-Intermediate Software Development\Code\Assignments 2024 Spring\Assignment 1\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harsh\OneDrive\Desktop\Documents\rrc-ploytech\semi-2\ISD 2327 assignments\Assignment_1_harshdeep_bhinder\isd_project\tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECD6C5C-0BF7-4659-811B-1D416A6C1BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A006CBBA-7583-448E-9018-D7EFAC9EAEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D9DD509-55B1-455D-8036-16809AD15960}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -270,7 +270,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1087,9 +1087,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADEBCC4-BB44-48CD-B9AB-1E2FD3EE0EEB}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.7109375" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
@@ -1099,8 +1101,8 @@
     <col min="7" max="7" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1"/>
-    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="1.45">
       <c r="B2" s="2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
@@ -1112,14 +1114,14 @@
       <c r="F2" s="13"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1">
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="15"/>
       <c r="D3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1128,10 +1130,10 @@
       </c>
       <c r="D4" s="18"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="10" t="s">
         <v>4</v>
       </c>
@@ -1151,7 +1153,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="66" customHeight="1">
+    <row r="7" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="9">
         <v>1</v>
@@ -1166,7 +1168,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" ht="66" customHeight="1">
+    <row r="8" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="11">
         <v>2</v>
@@ -1181,7 +1183,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:7" ht="66" customHeight="1">
+    <row r="9" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="11">
         <v>3</v>
@@ -1196,7 +1198,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:7" ht="66" customHeight="1">
+    <row r="10" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="9">
         <v>4</v>
@@ -1211,7 +1213,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:7" ht="66" customHeight="1">
+    <row r="11" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="11">
         <v>5</v>
@@ -1226,7 +1228,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:7" ht="31.15" customHeight="1">
+    <row r="12" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="11">
         <v>6</v>
       </c>
@@ -1240,7 +1242,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:7" ht="31.15" customHeight="1">
+    <row r="13" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="9">
         <v>7</v>
       </c>
@@ -1254,7 +1256,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:7" ht="31.15" customHeight="1">
+    <row r="14" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="11">
         <v>8</v>
       </c>
@@ -1268,7 +1270,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:7" ht="31.15" customHeight="1">
+    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="11">
         <v>9</v>
       </c>
@@ -1282,7 +1284,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:7" ht="31.15" customHeight="1">
+    <row r="16" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="9">
         <v>10</v>
       </c>
@@ -1296,7 +1298,7 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="2:7" ht="31.15" customHeight="1">
+    <row r="17" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="11">
         <v>11</v>
       </c>
@@ -1306,7 +1308,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="2:7" ht="31.15" customHeight="1">
+    <row r="18" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="11">
         <v>12</v>
       </c>
@@ -1316,7 +1318,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="2:7" ht="31.15" customHeight="1">
+    <row r="19" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="9">
         <v>13</v>
       </c>
@@ -1326,7 +1328,7 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="2:7" ht="31.15" customHeight="1">
+    <row r="20" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="11">
         <v>14</v>
       </c>
@@ -1336,7 +1338,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="2:7" ht="31.15" customHeight="1">
+    <row r="21" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="11">
         <v>15</v>
       </c>
@@ -1346,7 +1348,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="2:7" ht="31.15" customHeight="1">
+    <row r="22" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="9">
         <v>16</v>
       </c>
@@ -1356,7 +1358,7 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="2:7" ht="31.15" customHeight="1">
+    <row r="23" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="11">
         <v>17</v>
       </c>
@@ -1366,7 +1368,7 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="2:7" ht="31.15" customHeight="1">
+    <row r="24" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="11">
         <v>18</v>
       </c>
@@ -1376,7 +1378,7 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="2:7" ht="31.15" customHeight="1">
+    <row r="25" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9">
         <v>19</v>
       </c>
@@ -1386,7 +1388,7 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="2:7" ht="31.15" customHeight="1">
+    <row r="26" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="11">
         <v>20</v>
       </c>
@@ -1396,7 +1398,7 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="2:7" ht="31.15" customHeight="1">
+    <row r="27" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="11">
         <v>21</v>
       </c>
@@ -1406,7 +1408,7 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="2:7" ht="31.15" customHeight="1">
+    <row r="28" spans="2:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="9">
         <v>22</v>
       </c>
@@ -1416,7 +1418,7 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="30" spans="2:7">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="19" t="s">
         <v>26</v>
       </c>

</xml_diff>